<commit_message>
Added SVM V3 with 82% accuracy
</commit_message>
<xml_diff>
--- a/DEVELOPMENT SVM/SVM with LBP.xlsx
+++ b/DEVELOPMENT SVM/SVM with LBP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BSD-Detection\DEVELOPMENT SVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B51E6A-B83D-40A0-886B-58A412DB8785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE564E59-6746-4902-9BE9-2972F1ECF89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14760" yWindow="1290" windowWidth="12825" windowHeight="11295" xr2:uid="{F3E9132B-6B90-4C06-91FB-1840601734CE}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,10 +564,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -773,10 +773,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>